<commit_message>
Updates following Fevik meeting
</commit_message>
<xml_diff>
--- a/tidied_data_series/martini_river_outlets.xlsx
+++ b/tidied_data_series/martini_river_outlets.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED48BB8-E1CA-44C9-97E7-A3C8887C4963}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rivers" sheetId="1" r:id="rId1"/>
@@ -366,11 +367,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +390,13 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -412,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -453,10 +461,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -733,11 +744,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -752,7 +763,7 @@
     <col min="8" max="8" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1">
+    <row r="1" spans="1:11" s="7" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>81</v>
       </c>
@@ -778,7 +789,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>34</v>
       </c>
@@ -795,7 +806,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>35</v>
       </c>
@@ -812,7 +823,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>36</v>
       </c>
@@ -829,7 +840,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>37</v>
       </c>
@@ -837,16 +848,17 @@
         <v>61</v>
       </c>
       <c r="F5" s="2">
-        <v>57.592199999999998</v>
+        <v>57.595284999999997</v>
       </c>
       <c r="G5" s="2">
-        <v>10.149800000000001</v>
+        <v>10.170325999999999</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>38</v>
       </c>
@@ -863,7 +875,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>39</v>
       </c>
@@ -880,7 +892,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>40</v>
       </c>
@@ -897,7 +909,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>41</v>
       </c>
@@ -914,7 +926,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>42</v>
       </c>
@@ -931,7 +943,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -954,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -978,7 +990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1026,7 +1038,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1049,7 +1061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -1702,7 +1714,7 @@
       <c r="G44" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H44"/>
+  <autoFilter ref="A1:H44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>